<commit_message>
Second set of updates for PL
</commit_message>
<xml_diff>
--- a/input/scenario_parametricMatching.xlsx
+++ b/input/scenario_parametricMatching.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPaths_HU\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A1C58E-5CFF-44B2-8293-F316E20A7BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D494190-CD92-4B9D-8FAA-645B0D9CB41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17385" yWindow="2160" windowWidth="21480" windowHeight="12675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="UK" sheetId="1" r:id="rId1"/>
-    <sheet name="IT" sheetId="2" r:id="rId2"/>
-    <sheet name="HU" sheetId="3" r:id="rId3"/>
+    <sheet name="PL" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Parameter</t>
   </si>
@@ -371,139 +369,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>1.997664543524416</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>3.5955856795675567</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>22.576468464147236</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>128.43670192455068</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>0.80599803083943655</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F776AA79-ABB4-4A2A-AA34-CAA220F4565A}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>2.19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>6.51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>29.95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>17.309999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>5.34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444B2324-3054-412E-8905-C102B14CD321}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5769AF8-62B2-4A3A-B6B7-FA352FF4E890}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" style="1" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -520,7 +393,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>2.6102797657774888</v>
+        <v>2.1381718797449136</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -528,7 +401,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>0.59364273905668574</v>
+        <v>0.60782764497165009</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -536,7 +409,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>18.630588957020148</v>
+        <v>13.104739744807855</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -544,7 +417,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>6.5924098256054133</v>
+        <v>10.816036303272808</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -552,7 +425,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>0.14065686203904415</v>
+        <v>0.51751946378299496</v>
       </c>
     </row>
   </sheetData>

</xml_diff>